<commit_message>
updated README.md and project documentation(project plan)
</commit_message>
<xml_diff>
--- a/Documentation/jwtauth-project-plan.xlsx
+++ b/Documentation/jwtauth-project-plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\JwtAuth\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A83706-3651-4E4E-9C15-D0FD0784F7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225630B3-D88F-413E-A20D-56A342F14454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{90926BA7-FADE-4756-91C2-609B736D4DEF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="67">
   <si>
     <t>Project</t>
   </si>
@@ -325,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -338,7 +338,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -693,10 +694,10 @@
   <dimension ref="B3:D62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C32" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C44" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
+      <selection pane="bottomRight" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1159,61 +1160,73 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B44" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="5" t="s">
+    <row r="44" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="8"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B45" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="D44" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="8"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="5" t="s">
+      <c r="D45" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="8"/>
+      <c r="D46" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="47" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B47" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" s="4" t="s">
+      <c r="B47" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="6"/>
+      <c r="D47" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="48" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="4" t="s">
+      <c r="B48" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D48" s="6"/>
+      <c r="D48" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="49" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C49" s="4" t="s">
+      <c r="B49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D49" s="6"/>
-    </row>
-    <row r="50" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D49" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" s="4" t="s">
         <v>25</v>
       </c>
@@ -1222,7 +1235,7 @@
       </c>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" s="4" t="s">
         <v>25</v>
       </c>
@@ -1231,7 +1244,7 @@
       </c>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" s="4" t="s">
         <v>25</v>
       </c>
@@ -1240,7 +1253,7 @@
       </c>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" s="4" t="s">
         <v>25</v>
       </c>
@@ -1249,7 +1262,7 @@
       </c>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" s="4" t="s">
         <v>25</v>
       </c>
@@ -1258,7 +1271,7 @@
       </c>
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" s="4" t="s">
         <v>25</v>
       </c>
@@ -1267,7 +1280,7 @@
       </c>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" s="4" t="s">
         <v>25</v>
       </c>
@@ -1276,7 +1289,7 @@
       </c>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="4" t="s">
         <v>25</v>
       </c>
@@ -1285,7 +1298,7 @@
       </c>
       <c r="D57" s="6"/>
     </row>
-    <row r="58" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" s="4" t="s">
         <v>25</v>
       </c>
@@ -1294,7 +1307,7 @@
       </c>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" s="4" t="s">
         <v>25</v>
       </c>
@@ -1303,7 +1316,7 @@
       </c>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" s="4" t="s">
         <v>25</v>
       </c>
@@ -1312,7 +1325,7 @@
       </c>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" s="4" t="s">
         <v>25</v>
       </c>
@@ -1321,7 +1334,7 @@
       </c>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="2:4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" s="4" t="s">
         <v>25</v>
       </c>
@@ -1332,9 +1345,6 @@
     </row>
   </sheetData>
   <autoFilter ref="B3:D62" xr:uid="{C33C3F01-8269-4E57-9749-99DE44E2CF5B}">
-    <filterColumn colId="1">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>